<commit_message>
add shopping mall price and title xpath
</commit_message>
<xml_diff>
--- a/shopping_mall_page_info.xlsx
+++ b/shopping_mall_page_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\befly\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\befly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1522C5E-7D32-41EA-83C1-A5198683E286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AD1A45-FC4C-4F4A-9755-C89E304A8EE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A2EF0613-A5B6-4E3A-8E9E-A4B5AB4F053D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>사이트 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,14 +47,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상품명 class name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가격 class name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>티몬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -67,7 +59,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tx</t>
+    <t>상품명 Xpath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격 Xpath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//div[@class='price_area']/span[@class='price']/span[@class='sale']/i[@class='num']</t>
+  </si>
+  <si>
+    <t>//div[@class='deal_info']/p[@class='title']/strong[@class='tx']</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -132,7 +135,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -141,6 +144,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -459,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF3939-304F-4EA5-9546-E3CF9C494753}">
   <dimension ref="C2:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -468,8 +474,8 @@
     <col min="3" max="3" width="11.08203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.9140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="74.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.45">
@@ -483,23 +489,26 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
       <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add min-max price and loading method
</commit_message>
<xml_diff>
--- a/shopping_mall_page_info.xlsx
+++ b/shopping_mall_page_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\befly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\befly\wannaKnowMarketPrice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AD1A45-FC4C-4F4A-9755-C89E304A8EE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E13A803-F917-4A32-B04B-C74064AF7C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A2EF0613-A5B6-4E3A-8E9E-A4B5AB4F053D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>사이트 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>?keyword=</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상품명 Xpath</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,6 +67,26 @@
   </si>
   <si>
     <t>//div[@class='deal_info']/p[@class='title']/strong[@class='tx']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최소, 최대 금액 변수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;commonFilters=minPrice:{금액},maxPrice:{금액}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?keyword={검색어}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음 페이지 로드 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동 스크롤: browser.execute_script("window.scrollTo(0, document.body.scrollHeight);")</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -463,22 +479,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF3939-304F-4EA5-9546-E3CF9C494753}">
-  <dimension ref="C2:G3"/>
+  <dimension ref="C2:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="11.08203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="74.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="78.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,13 +507,19 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -503,13 +527,19 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>8</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add NAVER Shopping information, add 'parent element Xpath' column
</commit_message>
<xml_diff>
--- a/shopping_mall_page_info.xlsx
+++ b/shopping_mall_page_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\befly\wannaKnowMarketPrice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E13A803-F917-4A32-B04B-C74064AF7C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31405D98-FD4C-4DA9-828C-159BCEAF14AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A2EF0613-A5B6-4E3A-8E9E-A4B5AB4F053D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>사이트 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,13 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>//div[@class='price_area']/span[@class='price']/span[@class='sale']/i[@class='num']</t>
-  </si>
-  <si>
-    <t>//div[@class='deal_info']/p[@class='title']/strong[@class='tx']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>최소, 최대 금액 변수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -87,6 +80,54 @@
   </si>
   <si>
     <t>자동 스크롤: browser.execute_script("window.scrollTo(0, document.body.scrollHeight);")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버쇼핑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/search/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all.nhn?query={검색어}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용 불가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부모 노드 Xpath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//*[@id="_search_list"]/div[1]/ul/li/div[@class='info']/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./div[@class='price_area']/span[@class='price']/span[@class='sale']/i[@class='num']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./div[@class='tit']/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./span[@class='price']/em/span[@class='num _price_reload'] OR, span[@class='price']/em/span[@class='num']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[todo] 추가하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//*[@id='search_app']/div[2]/section/div/ul/div/div/li/a/div[3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./p[@class='title']/strong[@class='tx']</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -479,24 +520,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF3939-304F-4EA5-9546-E3CF9C494753}">
-  <dimension ref="C2:I3"/>
+  <dimension ref="C2:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="78.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="75.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -507,19 +549,22 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -527,27 +572,57 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>7</v>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{340D00D5-1F3B-4489-A98B-310946BE6D4F}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{3CB543E8-865B-4AF6-8761-62F1927EAC87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>